<commit_message>
TI complet + TVML
</commit_message>
<xml_diff>
--- a/Теория вероятности и математическая статистика/TVML.xlsx
+++ b/Теория вероятности и математическая статистика/TVML.xlsx
@@ -62,6 +62,188 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$J$5:$S$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$J$6:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="69164416"/>
+        <c:axId val="69301376"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="69164416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69301376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69301376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69164416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,38 +531,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:H14"/>
+  <dimension ref="A5:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="R5" sqref="R5:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:19">
       <c r="H5">
         <f>1/10</f>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5">
+        <v>-1</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>10</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+      <c r="S5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="H6">
         <f>729/1000</f>
         <v>0.72899999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0.2</v>
+      </c>
+      <c r="M6">
+        <v>0.2</v>
+      </c>
+      <c r="N6">
+        <v>0.1</v>
+      </c>
+      <c r="O6">
+        <v>0.1</v>
+      </c>
+      <c r="P6">
+        <v>0.4</v>
+      </c>
+      <c r="Q6">
+        <v>0.4</v>
+      </c>
+      <c r="R6">
+        <v>0.3</v>
+      </c>
+      <c r="S6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="H7">
         <f>H5*H6</f>
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:19">
       <c r="D9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -403,7 +645,7 @@
         <v>0.29160000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>0.05</v>
       </c>
@@ -426,7 +668,7 @@
         <v>4.8600000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>0.08</v>
       </c>
@@ -446,13 +688,13 @@
         <v>3.6000000000000003E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:19">
       <c r="H13">
         <f>1*0.0001*1</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:19">
       <c r="B14">
         <f>A11*B12+A12*B11</f>
         <v>0.122</v>
@@ -460,5 +702,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>